<commit_message>
2014 is completely clean!!!!
</commit_message>
<xml_diff>
--- a/errorsfixed_elise.xlsx
+++ b/errorsfixed_elise.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9CB7B7-9CDF-ED43-9713-9140295E56AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF5957E-75A8-4D49-A89B-62CCAB4EB0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{447D1116-2E76-DA4F-8A39-623521835E0C}"/>
+    <workbookView xWindow="-37920" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{447D1116-2E76-DA4F-8A39-623521835E0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Record_year</t>
   </si>
@@ -95,16 +95,13 @@
     <t>multiple</t>
   </si>
   <si>
-    <t>412C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obs date 2 days after last record </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/17/2014 verified as correct date so update last record to the 17th </t>
-  </si>
-  <si>
-    <t>404C2</t>
+    <t>401A</t>
+  </si>
+  <si>
+    <t>Month is 24, day is 3 theyre flipped</t>
+  </si>
+  <si>
+    <t>make month 3 and day 24</t>
   </si>
 </sst>
 </file>
@@ -140,8 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F28C52-5F00-1042-AF1D-AE82EC61F45A}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,32 +563,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>2014</v>
       </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>2014</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C27">
-        <v>205</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C12">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E12" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L26" s="1">
+        <v>41720</v>
+      </c>
+      <c r="M26" s="1">
+        <f>L26+27</f>
+        <v>41747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created analysis rmd, cleaned 2018 (remove NAs and pick columns still), covariate 2014 data also needs to be added
</commit_message>
<xml_diff>
--- a/errorsfixed_elise.xlsx
+++ b/errorsfixed_elise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF5957E-75A8-4D49-A89B-62CCAB4EB0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB01B325-D7FE-B840-8B0E-E210C8BBE911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37920" yWindow="500" windowWidth="28040" windowHeight="16540" xr2:uid="{447D1116-2E76-DA4F-8A39-623521835E0C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{447D1116-2E76-DA4F-8A39-623521835E0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Record_year</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>make month 3 and day 24</t>
+  </si>
+  <si>
+    <t>801C</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,6 +566,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2018</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>5129</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2014</v>

</xml_diff>

<commit_message>
need to go through 2019 again - before errors 134 (seems dates are wrong for cam - go to pictures and use first and last pic )
</commit_message>
<xml_diff>
--- a/errorsfixed_elise.xlsx
+++ b/errorsfixed_elise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB01B325-D7FE-B840-8B0E-E210C8BBE911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFD0DBC-04A2-254B-82AB-66B99D894A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{447D1116-2E76-DA4F-8A39-623521835E0C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Record_year</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>801C</t>
+  </si>
+  <si>
+    <t>907E</t>
+  </si>
+  <si>
+    <t>one day off in last record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some should be 2020 not 2019 </t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,6 +586,22 @@
         <v>5129</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2014</v>

</xml_diff>